<commit_message>
tabella training inizio work
</commit_message>
<xml_diff>
--- a/tabella_training.xlsx
+++ b/tabella_training.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\151588\Desktop\Simo\Waste Collection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\wm-stochastic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2453044A-EB89-4CB4-A97E-93A39453E707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761201AA-616C-4FA2-A286-C4F1C3725903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,56 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>DEPOT LOCATION</t>
-  </si>
-  <si>
-    <t>corner/central</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deviation distances from the depot </t>
-  </si>
-  <si>
-    <t>DISPERSION CUST</t>
-  </si>
-  <si>
-    <t>DISPERSION DIST</t>
-  </si>
-  <si>
-    <t>deviation distances from the gravity center (no depot)</t>
-  </si>
-  <si>
-    <t>% PATTERN SCHOOL</t>
-  </si>
-  <si>
-    <t>% PATTERN HOME</t>
-  </si>
-  <si>
-    <t>% PATTERN RESTAURANT</t>
-  </si>
-  <si>
-    <t>EXPECTED DEMAND / TOTAL CAPACITY</t>
-  </si>
-  <si>
-    <t>INITIAL DEMAND / TOTAL CAPACITY</t>
-  </si>
-  <si>
-    <t>TIMESLOT SIZE</t>
-  </si>
-  <si>
-    <t>{5,10,15}</t>
-  </si>
-  <si>
-    <t># CUSTOMERS</t>
-  </si>
-  <si>
-    <t># VEHICLES</t>
-  </si>
-  <si>
     <t>P1</t>
   </si>
   <si>
@@ -109,6 +64,39 @@
   </si>
   <si>
     <t>P12</t>
+  </si>
+  <si>
+    <t>initial_demand_on_tot_capacity</t>
+  </si>
+  <si>
+    <t>time_slot_size</t>
+  </si>
+  <si>
+    <t>expected_demand_on_tot_capacity</t>
+  </si>
+  <si>
+    <t>n_customers</t>
+  </si>
+  <si>
+    <t>n_vehicles</t>
+  </si>
+  <si>
+    <t>depot_location</t>
+  </si>
+  <si>
+    <t>dispersion_customers</t>
+  </si>
+  <si>
+    <t>dispersion_distance_depot</t>
+  </si>
+  <si>
+    <t>perc_pattern_school</t>
+  </si>
+  <si>
+    <t>perc_pattern_home</t>
+  </si>
+  <si>
+    <t>perc_pattern_restaurant</t>
   </si>
 </sst>
 </file>
@@ -431,113 +419,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
     <col min="2" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
-    <col min="9" max="9" width="24.44140625" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" customWidth="1"/>
-    <col min="11" max="11" width="35.5546875" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" customWidth="1"/>
+    <col min="11" max="11" width="35.5703125" customWidth="1"/>
     <col min="12" max="12" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>13</v>
-      </c>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L2" s="1"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E12" s="1"/>
     </row>
   </sheetData>

</xml_diff>